<commit_message>
Minor edits to templates
</commit_message>
<xml_diff>
--- a/templates/Plasmodium/NOMADS_Library_Ligation_Plasmo_Worksheet.xlsx
+++ b/templates/Plasmodium/NOMADS_Library_Ligation_Plasmo_Worksheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\templates\Plasmodium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitrepos\warehouse\templates\Plasmodium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA4650B-D4D4-496C-A015-E4880702AF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81111B7-55AB-4952-B811-FD7E3A7B4393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2488,37 +2488,100 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2533,88 +2596,25 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -3503,7 +3503,7 @@
   </sheetPr>
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
@@ -3513,171 +3513,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="121" t="s">
         <v>418</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="90" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="J2" s="91" t="s">
+      <c r="H2" s="104"/>
+      <c r="J2" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="91"/>
+      <c r="K2" s="123"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
       <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="93" t="s">
+      <c r="J3" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="93"/>
+      <c r="K3" s="125"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
       <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="94" t="s">
+      <c r="J4" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="94"/>
+      <c r="K4" s="126"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="96" t="str">
+      <c r="B5" s="116"/>
+      <c r="C5" s="102" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!H3:I9,2,FALSE()),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="97"/>
+      <c r="K5" s="117"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="98" t="str">
+      <c r="B6" s="116"/>
+      <c r="C6" s="118" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
       <c r="G6" s="5"/>
-      <c r="J6" s="97"/>
-      <c r="K6" s="97"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="99"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
       <c r="G7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="99"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="101" t="s">
+      <c r="A9" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="102" t="str">
+      <c r="B9" s="112"/>
+      <c r="C9" s="113" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="102" t="str">
+      <c r="B10" s="112"/>
+      <c r="C10" s="113" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="102"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="88" t="s">
+      <c r="A11" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="88"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="27"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -3685,32 +3685,32 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="114"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="114"/>
+      <c r="I12" s="114"/>
+      <c r="J12" s="114"/>
+      <c r="K12" s="114"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="103"/>
-      <c r="J13" s="103"/>
-      <c r="K13" s="103"/>
+      <c r="C13" s="114"/>
+      <c r="D13" s="114"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="6"/>
@@ -3721,11 +3721,11 @@
       </c>
       <c r="C15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="I15" s="104" t="s">
+      <c r="I15" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="104"/>
-      <c r="K15" s="104"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="115"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -3755,119 +3755,119 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="105" t="s">
+      <c r="A18" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="105"/>
-      <c r="C18" s="105"/>
-      <c r="D18" s="106" t="s">
+      <c r="B18" s="98"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106" t="str">
+      <c r="E18" s="111"/>
+      <c r="F18" s="111" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G18" s="106"/>
-      <c r="I18" s="107" t="s">
+      <c r="G18" s="111"/>
+      <c r="I18" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="107"/>
+      <c r="J18" s="91"/>
       <c r="K18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="108" t="s">
+      <c r="A19" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="108"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="109" t="s">
+      <c r="B19" s="95"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="109"/>
-      <c r="F19" s="110" t="s">
+      <c r="E19" s="106"/>
+      <c r="F19" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="110"/>
-      <c r="I19" s="111">
+      <c r="G19" s="107"/>
+      <c r="I19" s="101">
         <v>20</v>
       </c>
-      <c r="J19" s="111"/>
+      <c r="J19" s="101"/>
       <c r="K19" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="108" t="s">
+      <c r="A20" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="108"/>
-      <c r="C20" s="108"/>
-      <c r="D20" s="109" t="str">
+      <c r="B20" s="95"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="106" t="str">
         <f>CONCATENATE(endrepair_maxvol, " - x")</f>
         <v>10 - x</v>
       </c>
-      <c r="E20" s="109"/>
-      <c r="F20" s="110" t="s">
+      <c r="E20" s="106"/>
+      <c r="F20" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="110"/>
-      <c r="I20" s="111">
+      <c r="G20" s="107"/>
+      <c r="I20" s="101">
         <v>65</v>
       </c>
-      <c r="J20" s="111"/>
+      <c r="J20" s="101"/>
       <c r="K20" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="3" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="108" t="s">
+      <c r="A21" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="108"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="112">
+      <c r="B21" s="95"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="109">
         <v>1.4</v>
       </c>
-      <c r="E21" s="112"/>
-      <c r="F21" s="110">
+      <c r="E21" s="109"/>
+      <c r="F21" s="107">
         <f>SUM(D21*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="110"/>
-      <c r="I21" s="111">
+      <c r="G21" s="107"/>
+      <c r="I21" s="101">
         <v>4</v>
       </c>
-      <c r="J21" s="111"/>
+      <c r="J21" s="101"/>
       <c r="K21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="108" t="s">
+      <c r="A22" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="108"/>
-      <c r="C22" s="108"/>
-      <c r="D22" s="112">
+      <c r="B22" s="95"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="109">
         <v>0.6</v>
       </c>
-      <c r="E22" s="112"/>
-      <c r="F22" s="110">
+      <c r="E22" s="109"/>
+      <c r="F22" s="107">
         <f>SUM(D22*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="110"/>
+      <c r="G22" s="107"/>
     </row>
     <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="D23" s="113">
+      <c r="D23" s="110">
         <f>SUM(D21:D22)+endrepair_maxvol</f>
         <v>12</v>
       </c>
-      <c r="E23" s="113"/>
+      <c r="E23" s="110"/>
       <c r="F23" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D21:D22)," µl of MM to each")</f>
         <v>Add 2 µl of MM to each</v>
@@ -3892,103 +3892,103 @@
       </c>
     </row>
     <row r="26" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="105" t="s">
+      <c r="A26" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="105"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="106" t="s">
+      <c r="B26" s="98"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="106"/>
-      <c r="F26" s="106" t="str">
+      <c r="E26" s="111"/>
+      <c r="F26" s="111" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G26" s="106"/>
-      <c r="I26" s="107" t="s">
+      <c r="G26" s="111"/>
+      <c r="I26" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="107"/>
+      <c r="J26" s="91"/>
       <c r="K26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="108" t="s">
+      <c r="A27" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="108"/>
-      <c r="C27" s="108"/>
-      <c r="D27" s="109">
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="106">
         <v>0.5</v>
       </c>
-      <c r="E27" s="109"/>
-      <c r="F27" s="110" t="s">
+      <c r="E27" s="106"/>
+      <c r="F27" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="110"/>
-      <c r="I27" s="111">
+      <c r="G27" s="107"/>
+      <c r="I27" s="101">
         <v>20</v>
       </c>
-      <c r="J27" s="111"/>
+      <c r="J27" s="101"/>
       <c r="K27" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="108" t="s">
+      <c r="A28" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="108"/>
-      <c r="C28" s="108"/>
-      <c r="D28" s="109">
+      <c r="B28" s="95"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="106">
         <v>6</v>
       </c>
-      <c r="E28" s="109"/>
-      <c r="F28" s="110">
+      <c r="E28" s="106"/>
+      <c r="F28" s="107">
         <f>SUM(D28*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="110"/>
-      <c r="I28" s="111">
+      <c r="G28" s="107"/>
+      <c r="I28" s="101">
         <v>65</v>
       </c>
-      <c r="J28" s="111"/>
+      <c r="J28" s="101"/>
       <c r="K28" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="108" t="s">
+      <c r="A29" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="108"/>
-      <c r="C29" s="108"/>
-      <c r="D29" s="109">
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="106">
         <v>0.2</v>
       </c>
-      <c r="E29" s="109"/>
-      <c r="F29" s="110">
+      <c r="E29" s="106"/>
+      <c r="F29" s="107">
         <f>SUM(D29*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G29" s="110"/>
-      <c r="I29" s="111">
+      <c r="G29" s="107"/>
+      <c r="I29" s="101">
         <v>8</v>
       </c>
-      <c r="J29" s="111"/>
+      <c r="J29" s="101"/>
       <c r="K29" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="D30" s="114">
+      <c r="D30" s="108">
         <f>SUM(D27:D29)+D23</f>
         <v>18.7</v>
       </c>
-      <c r="E30" s="114"/>
+      <c r="E30" s="108"/>
       <c r="F30" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D28:D29)," µl of MM to each")</f>
         <v>Add 6.2 µl of MM to each</v>
@@ -4012,20 +4012,20 @@
       <c r="G33" s="26"/>
     </row>
     <row r="34" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="90"/>
-      <c r="C34" s="90"/>
-      <c r="D34" s="90"/>
-      <c r="E34" s="90"/>
-      <c r="F34" s="90"/>
-      <c r="G34" s="90"/>
-      <c r="H34" s="90"/>
-      <c r="I34" s="90"/>
-      <c r="J34" s="90"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
+      <c r="B34" s="104"/>
+      <c r="C34" s="104"/>
+      <c r="D34" s="104"/>
+      <c r="E34" s="104"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="104"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
+      <c r="K34" s="104"/>
+      <c r="L34" s="104"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
@@ -4048,10 +4048,10 @@
       <c r="C36" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="115" t="s">
+      <c r="D36" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="115"/>
+      <c r="E36" s="93"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
@@ -4060,11 +4060,11 @@
       </c>
       <c r="B37" s="34"/>
       <c r="C37" s="34"/>
-      <c r="D37" s="116">
+      <c r="D37" s="105">
         <f>SUM(B37*C37)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="116"/>
+      <c r="E37" s="105"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -4086,97 +4086,97 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="107" t="s">
+      <c r="A41" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="107"/>
-      <c r="C41" s="107"/>
-      <c r="D41" s="117" t="s">
+      <c r="B41" s="91"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="117"/>
-      <c r="I41" s="107" t="s">
+      <c r="E41" s="92"/>
+      <c r="I41" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="J41" s="107"/>
+      <c r="J41" s="91"/>
       <c r="K41" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="108" t="s">
+      <c r="A42" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="108"/>
-      <c r="C42" s="108"/>
-      <c r="D42" s="118">
+      <c r="B42" s="95"/>
+      <c r="C42" s="95"/>
+      <c r="D42" s="94">
         <f>IF(B37="",adaptlig_dna_maxvol,IF(SUM(adaptlig_targetmass/D37)&gt;adaptlig_dna_maxvol,adaptlig_dna_maxvol,SUM(adaptlig_targetmass/D37)))</f>
         <v>30</v>
       </c>
-      <c r="E42" s="118"/>
+      <c r="E42" s="94"/>
       <c r="F42" s="5"/>
-      <c r="I42" s="111" t="s">
+      <c r="I42" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="J42" s="111"/>
+      <c r="J42" s="101"/>
       <c r="K42" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="108" t="s">
+      <c r="A43" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="108"/>
-      <c r="C43" s="108"/>
-      <c r="D43" s="118">
+      <c r="B43" s="95"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="94">
         <f>IFERROR(SUM(adaptlig_dna_maxvol-D42),"")</f>
         <v>0</v>
       </c>
-      <c r="E43" s="118"/>
+      <c r="E43" s="94"/>
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="108" t="s">
+      <c r="A44" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="108"/>
-      <c r="C44" s="108"/>
-      <c r="D44" s="96">
+      <c r="B44" s="95"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="102">
         <v>5</v>
       </c>
-      <c r="E44" s="96"/>
+      <c r="E44" s="102"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="108" t="s">
+      <c r="A45" s="95" t="s">
         <v>406</v>
       </c>
-      <c r="B45" s="108"/>
-      <c r="C45" s="108"/>
-      <c r="D45" s="96">
+      <c r="B45" s="95"/>
+      <c r="C45" s="95"/>
+      <c r="D45" s="102">
         <f>SUM(adaptlig_rxn_vol/5)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="96"/>
+      <c r="E45" s="102"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="108" t="s">
+      <c r="A46" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="108"/>
-      <c r="C46" s="108"/>
-      <c r="D46" s="96">
+      <c r="B46" s="95"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="102">
         <f>SUM(adaptlig_rxn_vol/10)</f>
         <v>0</v>
       </c>
-      <c r="E46" s="96"/>
+      <c r="E46" s="102"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D47" s="119">
+      <c r="D47" s="103">
         <f>SUM(D42:D46)</f>
         <v>35</v>
       </c>
-      <c r="E47" s="119"/>
+      <c r="E47" s="103"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
@@ -4193,20 +4193,20 @@
       <c r="J50" s="47"/>
     </row>
     <row r="51" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="120" t="s">
+      <c r="A51" s="97" t="s">
         <v>413</v>
       </c>
-      <c r="B51" s="120"/>
-      <c r="C51" s="120"/>
-      <c r="D51" s="120"/>
-      <c r="E51" s="120"/>
-      <c r="F51" s="120"/>
-      <c r="G51" s="120"/>
-      <c r="H51" s="120"/>
-      <c r="I51" s="120"/>
-      <c r="J51" s="120"/>
-      <c r="K51" s="120"/>
-      <c r="L51" s="120"/>
+      <c r="B51" s="97"/>
+      <c r="C51" s="97"/>
+      <c r="D51" s="97"/>
+      <c r="E51" s="97"/>
+      <c r="F51" s="97"/>
+      <c r="G51" s="97"/>
+      <c r="H51" s="97"/>
+      <c r="I51" s="97"/>
+      <c r="J51" s="97"/>
+      <c r="K51" s="97"/>
+      <c r="L51" s="97"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
@@ -4220,38 +4220,38 @@
       <c r="G52" s="9"/>
     </row>
     <row r="53" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="105" t="s">
+      <c r="A53" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="105"/>
-      <c r="C53" s="105" t="s">
+      <c r="B53" s="98"/>
+      <c r="C53" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="105"/>
-      <c r="E53" s="105" t="s">
+      <c r="D53" s="98"/>
+      <c r="E53" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="F53" s="105"/>
-      <c r="G53" s="105" t="s">
+      <c r="F53" s="98"/>
+      <c r="G53" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="H53" s="105"/>
+      <c r="H53" s="98"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="121">
+      <c r="A54" s="99">
         <f>SUM(adaptlig_rxn_vol*0.5)</f>
         <v>0</v>
       </c>
-      <c r="B54" s="121"/>
-      <c r="C54" s="122"/>
-      <c r="D54" s="122"/>
-      <c r="E54" s="122"/>
-      <c r="F54" s="122"/>
-      <c r="G54" s="111">
+      <c r="B54" s="99"/>
+      <c r="C54" s="100"/>
+      <c r="D54" s="100"/>
+      <c r="E54" s="100"/>
+      <c r="F54" s="100"/>
+      <c r="G54" s="101">
         <f>SUM(C54*E54)</f>
         <v>0</v>
       </c>
-      <c r="H54" s="111"/>
+      <c r="H54" s="101"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
@@ -4270,61 +4270,61 @@
       <c r="H57" s="18"/>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="107" t="s">
+      <c r="A58" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B58" s="107"/>
-      <c r="C58" s="107"/>
-      <c r="D58" s="117" t="s">
+      <c r="B58" s="91"/>
+      <c r="C58" s="91"/>
+      <c r="D58" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="117"/>
+      <c r="E58" s="92"/>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="115" t="s">
+      <c r="A59" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="115"/>
-      <c r="C59" s="115"/>
-      <c r="D59" s="118">
+      <c r="B59" s="93"/>
+      <c r="C59" s="93"/>
+      <c r="D59" s="94">
         <f>IF(C54="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G54)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G54)))</f>
         <v>12</v>
       </c>
-      <c r="E59" s="118"/>
+      <c r="E59" s="94"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="115" t="s">
+      <c r="A60" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="115"/>
-      <c r="C60" s="115"/>
-      <c r="D60" s="118" t="str">
+      <c r="B60" s="93"/>
+      <c r="C60" s="93"/>
+      <c r="D60" s="94" t="str">
         <f>IFERROR((IF(SUM(12-D59)=0,"-",SUM(12-D59))),"")</f>
         <v>-</v>
       </c>
-      <c r="E60" s="118"/>
+      <c r="E60" s="94"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="108" t="s">
+      <c r="A61" s="95" t="s">
         <v>419</v>
       </c>
-      <c r="B61" s="108"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="123">
+      <c r="B61" s="95"/>
+      <c r="C61" s="95"/>
+      <c r="D61" s="96">
         <v>37.5</v>
       </c>
-      <c r="E61" s="123"/>
+      <c r="E61" s="96"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="108" t="s">
+      <c r="A62" s="95" t="s">
         <v>420</v>
       </c>
-      <c r="B62" s="108"/>
-      <c r="C62" s="108"/>
-      <c r="D62" s="123">
+      <c r="B62" s="95"/>
+      <c r="C62" s="95"/>
+      <c r="D62" s="96">
         <v>25.5</v>
       </c>
-      <c r="E62" s="123"/>
+      <c r="E62" s="96"/>
       <c r="F62" s="5" t="s">
         <v>58</v>
       </c>
@@ -4336,82 +4336,184 @@
       <c r="C64" s="5"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="88" t="s">
+      <c r="A65" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="B65" s="88"/>
-      <c r="C65" s="125"/>
-      <c r="D65" s="125"/>
+      <c r="B65" s="87"/>
+      <c r="C65" s="89"/>
+      <c r="D65" s="89"/>
       <c r="E65" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="88" t="s">
+      <c r="A66" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="B66" s="88"/>
-      <c r="C66" s="124"/>
-      <c r="D66" s="124"/>
+      <c r="B66" s="87"/>
+      <c r="C66" s="88"/>
+      <c r="D66" s="88"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="88" t="s">
+      <c r="A67" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="B67" s="88"/>
-      <c r="C67" s="124"/>
-      <c r="D67" s="124"/>
+      <c r="B67" s="87"/>
+      <c r="C67" s="88"/>
+      <c r="D67" s="88"/>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="88" t="s">
+      <c r="A68" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="B68" s="88"/>
-      <c r="C68" s="126" t="str">
+      <c r="B68" s="87"/>
+      <c r="C68" s="90" t="str">
         <f>IF(flowcell_status="New",0,"")</f>
         <v/>
       </c>
-      <c r="D68" s="126"/>
+      <c r="D68" s="90"/>
       <c r="E68" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="88" t="s">
+      <c r="A69" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="88"/>
-      <c r="C69" s="125"/>
-      <c r="D69" s="125"/>
+      <c r="B69" s="87"/>
+      <c r="C69" s="89"/>
+      <c r="D69" s="89"/>
       <c r="E69" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="88" t="s">
+      <c r="A70" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="88"/>
-      <c r="C70" s="124"/>
-      <c r="D70" s="124"/>
+      <c r="B70" s="87"/>
+      <c r="C70" s="88"/>
+      <c r="D70" s="88"/>
       <c r="E70" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="88" t="s">
+      <c r="A71" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="88"/>
-      <c r="C71" s="124"/>
-      <c r="D71" s="124"/>
+      <c r="B71" s="87"/>
+      <c r="C71" s="88"/>
+      <c r="D71" s="88"/>
       <c r="E71" s="9" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection sheet="1"/>
   <mergeCells count="116">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A51:L51"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D62:E62"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="A71:B71"/>
@@ -4426,108 +4528,6 @@
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="C69:D69"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A51:L51"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:K13"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="B57">
     <cfRule type="expression" dxfId="10" priority="2">
@@ -12790,9 +12790,7 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>